<commit_message>
Updating Video Pipeline code
</commit_message>
<xml_diff>
--- a/submissions.xlsx
+++ b/submissions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,42 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1233</t>
-        </is>
+      <c r="A3" t="n">
+        <v>1233</v>
       </c>
       <c r="B3" t="inlineStr">
+        <is>
+          <t>bus_driver.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>777</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>driver_class_demo.avi</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>344</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>driver_class_demo.avi</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>33333</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>bus_driver.mp4</t>
         </is>

</xml_diff>